<commit_message>
3-4 module, with ui, without education book
</commit_message>
<xml_diff>
--- a/import/user_import.xlsx
+++ b/import/user_import.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Новая папка (2)\Пример\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zh\Desktop\DemoExamenShoes\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D664F7-4F5D-45B1-932A-0A7FD83F7240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2136" windowWidth="26760" windowHeight="16560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Роль сотрудника</t>
   </si>
@@ -135,12 +130,15 @@
   </si>
   <si>
     <t>Авторизированный клиент</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -525,21 +523,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.796875" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
     <col min="2" max="2" width="38.5" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,8 +564,11 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -581,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -595,7 +596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -609,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -623,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -637,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -651,7 +652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -665,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -679,7 +680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -693,30 +694,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>